<commit_message>
Itens 1 e 2 terminados
</commit_message>
<xml_diff>
--- a/Exemplos.xlsx
+++ b/Exemplos.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Item 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Item 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Qual o sexo do cliente?</t>
   </si>
@@ -58,6 +57,57 @@
   </si>
   <si>
     <t>Valor pago aos cantores (que será 0 ou 3 reais)</t>
+  </si>
+  <si>
+    <t>Total de rendimentos bancarios</t>
+  </si>
+  <si>
+    <t>Total de rendimentos de salarios ou servicos</t>
+  </si>
+  <si>
+    <t>Total de outros rendimentos</t>
+  </si>
+  <si>
+    <t>Servicos medicos pagos</t>
+  </si>
+  <si>
+    <t>Servicos educacionais pagos</t>
+  </si>
+  <si>
+    <t>Total de impostos</t>
+  </si>
+  <si>
+    <t>sobre outros rendimentos</t>
+  </si>
+  <si>
+    <t>Total de valores possiveis de abater</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>serviços educacionais</t>
+  </si>
+  <si>
+    <t>serviços médicos</t>
+  </si>
+  <si>
+    <t>sobre salários serviços</t>
+  </si>
+  <si>
+    <t>sobre rendimentos bancários</t>
+  </si>
+  <si>
+    <t>Imposto total</t>
+  </si>
+  <si>
+    <t>imposto bruto</t>
+  </si>
+  <si>
+    <t>abatimentos</t>
+  </si>
+  <si>
+    <t>Máximo a ser abatido</t>
   </si>
 </sst>
 </file>
@@ -65,9 +115,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +140,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,8 +162,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,29 +192,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,177 +554,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="10">
         <f>IF(B2="M",10,8)</f>
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="10">
         <f>IF(C2="M",10,8)</f>
         <v>8</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="10">
         <f>IF(D2="M",10,8)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="10">
         <f>(B3*2.5)+(B4*2)+(B5*4)</f>
         <v>29</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <f>(C3*2.5)+(C4*2)+(C5*4)</f>
         <v>28.5</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="10">
         <f>(D3*2.5)+(D4*2)+(D5*4)</f>
-        <v>45.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="10">
         <f>IF(B8&lt;=15,3,0)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="10">
         <f>IF(C8&lt;=15,3,0)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="10">
         <f>IF(D8&lt;=15,3,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="10">
         <f>SUM(B7:B9)</f>
         <v>39</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="10">
         <f>SUM(C7:C9)</f>
         <v>36.5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="10">
         <f>SUM(D7:D9)</f>
-        <v>55.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="14">
         <f>B10*1.1</f>
         <v>42.900000000000006</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="14">
         <f>C10*1.1</f>
         <v>40.150000000000006</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="14">
         <f>D10*1.1</f>
-        <v>61.050000000000004</v>
+        <v>28.05</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D2">
-      <formula1>"M,F"</formula1>
+      <formula1>"M,m,F,f"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -633,24 +736,335 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="10">
+        <v>800</v>
+      </c>
+      <c r="D2" s="10">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10">
+        <v>15000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>7500</v>
+      </c>
+      <c r="D3" s="10">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10">
+        <v>880</v>
+      </c>
+      <c r="C4" s="10">
+        <v>400</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10">
+        <v>350</v>
+      </c>
+      <c r="C5" s="10">
+        <v>200</v>
+      </c>
+      <c r="D5" s="10">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="10">
+        <v>400</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10">
+        <f>B2*0.2</f>
+        <v>400</v>
+      </c>
+      <c r="C9" s="10">
+        <f t="shared" ref="C9:D9" si="0">C2*0.2</f>
+        <v>160</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10">
+        <f>IF(B3&lt;=8000,0,IF(AND(B3&gt;=8000.01,B3&lt;=24000),B3*0.15,IF(B3&gt;=24000.01,B3*0.2)))</f>
+        <v>2250</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" ref="C10:D10" si="1">IF(C3&lt;=8000,0,IF(AND(C3&gt;=8000.01,C3&lt;=24000),C3*0.15,IF(C3&gt;=24000.01,C3*0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="10">
+        <f>B4*0.1</f>
+        <v>88</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" ref="C11:D11" si="2">C4*0.1</f>
+        <v>40</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="2"/>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="10">
+        <f>SUM(B9:B11)</f>
+        <v>2738</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" ref="C12:D12" si="3">SUM(C9:C11)</f>
+        <v>200</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="3"/>
+        <v>5947</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="10">
+        <f>IF((B12*0.3)&lt;B19,B12*0.3,B19)</f>
+        <v>821.4</v>
+      </c>
+      <c r="C14" s="10">
+        <f t="shared" ref="C14:D14" si="4">IF((C12*0.3)&lt;C19,C12*0.3,C19)</f>
+        <v>60</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" si="4"/>
+        <v>1784.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="10">
+        <f>B5</f>
+        <v>350</v>
+      </c>
+      <c r="C17" s="10">
+        <f t="shared" ref="C17:D17" si="5">C5</f>
+        <v>200</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="5"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="10">
+        <f>B6</f>
+        <v>2000</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" ref="C18:D18" si="6">C6</f>
+        <v>400</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="6"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="10">
+        <f>SUM(B17:B18)</f>
+        <v>2350</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" ref="C19:D19" si="7">SUM(C17:C18)</f>
+        <v>600</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="7"/>
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="10">
+        <f>B12</f>
+        <v>2738</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" ref="C22:D22" si="8">C12</f>
+        <v>200</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="8"/>
+        <v>5947</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="10">
+        <f>B14</f>
+        <v>821.4</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" ref="C23:D23" si="9">C14</f>
+        <v>60</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="9"/>
+        <v>1784.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="13">
+        <f>B22-B23</f>
+        <v>1916.6</v>
+      </c>
+      <c r="C24" s="13">
+        <f t="shared" ref="C24:D24" si="10">C22-C23</f>
+        <v>140</v>
+      </c>
+      <c r="D24" s="13">
+        <f t="shared" si="10"/>
+        <v>4162.8999999999996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>